<commit_message>
refactor script to make it perfect
</commit_message>
<xml_diff>
--- a/src/main/java/ConfigData/ConfigData_UBNT_M2.xlsx
+++ b/src/main/java/ConfigData/ConfigData_UBNT_M2.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715"/>
   </bookViews>
   <sheets>
-    <sheet name="testData" sheetId="1" r:id="rId1"/>
+    <sheet name="ConfigData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -547,7 +547,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>

</xml_diff>